<commit_message>
3 noviembre, explicación de códigos
</commit_message>
<xml_diff>
--- a/Basededatos/ECC.xlsx
+++ b/Basededatos/ECC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{E1E9DAAB-6A72-4B92-9416-19E46066190C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C01EE179-B344-44B5-97BB-D1D3BF83FAA3}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{E1E9DAAB-6A72-4B92-9416-19E46066190C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B7439098-DFFB-45FE-8262-A475882708A8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{1994ACD4-0C07-4C23-B301-0329DFC64F6C}"/>
   </bookViews>
@@ -642,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -658,9 +658,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -799,13 +796,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -815,6 +805,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -831,7 +828,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE6815CF-2C80-4CC6-A2B3-AA82E91A050A}" name="Tabla1" displayName="Tabla1" ref="B2:D169" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE6815CF-2C80-4CC6-A2B3-AA82E91A050A}" name="Tabla1" displayName="Tabla1" ref="B2:D169" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="B2:D169" xr:uid="{52BA55F9-4ED9-4A6F-9660-03359BBFF6C5}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{373F01D6-B106-47AD-B02A-02B2683CC4BB}" name="SERIE" dataDxfId="2"/>
@@ -1142,7 +1139,7 @@
   <dimension ref="B2:D169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7:D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,13 +1148,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1201,7 +1198,7 @@
       <c r="C6" s="1">
         <v>45741</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>4</v>
       </c>
     </row>
@@ -1212,7 +1209,7 @@
       <c r="C7" s="1">
         <v>45741</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1223,7 +1220,7 @@
       <c r="C8" s="1">
         <v>45742</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1234,7 +1231,7 @@
       <c r="C9" s="1">
         <v>45743</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1245,7 +1242,7 @@
       <c r="C10" s="1">
         <v>45744</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1256,7 +1253,7 @@
       <c r="C11" s="1">
         <v>45745</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1267,7 +1264,7 @@
       <c r="C12" s="1">
         <v>45746</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1278,7 +1275,7 @@
       <c r="C13" s="1">
         <v>45747</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1289,7 +1286,7 @@
       <c r="C14" s="1">
         <v>45748</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1300,7 +1297,7 @@
       <c r="C15" s="1">
         <v>45749</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1311,7 +1308,7 @@
       <c r="C16" s="1">
         <v>45750</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1322,7 +1319,7 @@
       <c r="C17" s="1">
         <v>45751</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1333,7 +1330,7 @@
       <c r="C18" s="1">
         <v>45752</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1344,7 +1341,7 @@
       <c r="C19" s="1">
         <v>45753</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1355,7 +1352,7 @@
       <c r="C20" s="1">
         <v>45754</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1366,7 +1363,7 @@
       <c r="C21" s="1">
         <v>45755</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1377,7 +1374,7 @@
       <c r="C22" s="1">
         <v>45756</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1388,7 +1385,7 @@
       <c r="C23" s="1">
         <v>45757</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1399,7 +1396,7 @@
       <c r="C24" s="1">
         <v>45758</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1410,7 +1407,7 @@
       <c r="C25" s="1">
         <v>45759</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1421,7 +1418,7 @@
       <c r="C26" s="1">
         <v>45760</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1432,7 +1429,7 @@
       <c r="C27" s="1">
         <v>45761</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1443,7 +1440,7 @@
       <c r="C28" s="1">
         <v>45762</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1454,7 +1451,7 @@
       <c r="C29" s="1">
         <v>45763</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1465,7 +1462,7 @@
       <c r="C30" s="1">
         <v>45764</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1476,7 +1473,7 @@
       <c r="C31" s="1">
         <v>45765</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1487,7 +1484,7 @@
       <c r="C32" s="1">
         <v>45766</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1498,7 +1495,7 @@
       <c r="C33" s="1">
         <v>45767</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1509,7 +1506,7 @@
       <c r="C34" s="1">
         <v>45768</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1520,7 +1517,7 @@
       <c r="C35" s="1">
         <v>45769</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1531,7 +1528,7 @@
       <c r="C36" s="1">
         <v>45770</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1542,7 +1539,7 @@
       <c r="C37" s="1">
         <v>45771</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1553,7 +1550,7 @@
       <c r="C38" s="1">
         <v>45772</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1564,7 +1561,7 @@
       <c r="C39" s="1">
         <v>45773</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1575,7 +1572,7 @@
       <c r="C40" s="1">
         <v>45774</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1586,7 +1583,7 @@
       <c r="C41" s="1">
         <v>45775</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1597,7 +1594,7 @@
       <c r="C42" s="1">
         <v>45776</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1608,7 +1605,7 @@
       <c r="C43" s="1">
         <v>45777</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1619,7 +1616,7 @@
       <c r="C44" s="1">
         <v>45778</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1630,7 +1627,7 @@
       <c r="C45" s="1">
         <v>45779</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1641,7 +1638,7 @@
       <c r="C46" s="1">
         <v>45780</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1652,7 +1649,7 @@
       <c r="C47" s="1">
         <v>45781</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1663,7 +1660,7 @@
       <c r="C48" s="1">
         <v>45782</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1674,7 +1671,7 @@
       <c r="C49" s="1">
         <v>45783</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1685,7 +1682,7 @@
       <c r="C50" s="1">
         <v>45784</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1696,7 +1693,7 @@
       <c r="C51" s="1">
         <v>45785</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1707,7 +1704,7 @@
       <c r="C52" s="1">
         <v>45786</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1718,7 +1715,7 @@
       <c r="C53" s="1">
         <v>45787</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1729,7 +1726,7 @@
       <c r="C54" s="1">
         <v>45788</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1740,7 +1737,7 @@
       <c r="C55" s="1">
         <v>45789</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1751,7 +1748,7 @@
       <c r="C56" s="1">
         <v>45790</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1762,7 +1759,7 @@
       <c r="C57" s="1">
         <v>45791</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1773,7 +1770,7 @@
       <c r="C58" s="1">
         <v>45792</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1784,7 +1781,7 @@
       <c r="C59" s="1">
         <v>45793</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1795,7 +1792,7 @@
       <c r="C60" s="1">
         <v>45794</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1806,7 +1803,7 @@
       <c r="C61" s="1">
         <v>45795</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1817,7 +1814,7 @@
       <c r="C62" s="1">
         <v>45796</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1828,7 +1825,7 @@
       <c r="C63" s="1">
         <v>45797</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1839,7 +1836,7 @@
       <c r="C64" s="1">
         <v>45798</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1850,7 +1847,7 @@
       <c r="C65" s="1">
         <v>45799</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1861,7 +1858,7 @@
       <c r="C66" s="1">
         <v>45800</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1872,7 +1869,7 @@
       <c r="C67" s="1">
         <v>45801</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1883,7 +1880,7 @@
       <c r="C68" s="1">
         <v>45803</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1894,7 +1891,7 @@
       <c r="C69" s="1">
         <v>45804</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1905,7 +1902,7 @@
       <c r="C70" s="1">
         <v>45805</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1916,7 +1913,7 @@
       <c r="C71" s="1">
         <v>45806</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D71" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1927,7 +1924,7 @@
       <c r="C72" s="1">
         <v>45807</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D72" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1938,7 +1935,7 @@
       <c r="C73" s="1">
         <v>45808</v>
       </c>
-      <c r="D73" s="10">
+      <c r="D73" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1949,7 +1946,7 @@
       <c r="C74" s="1">
         <v>45809</v>
       </c>
-      <c r="D74" s="10">
+      <c r="D74" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1960,7 +1957,7 @@
       <c r="C75" s="1">
         <v>45810</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1971,7 +1968,7 @@
       <c r="C76" s="1">
         <v>45811</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1982,7 +1979,7 @@
       <c r="C77" s="1">
         <v>45812</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D77" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1993,7 +1990,7 @@
       <c r="C78" s="1">
         <v>45813</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D78" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2004,7 +2001,7 @@
       <c r="C79" s="1">
         <v>45814</v>
       </c>
-      <c r="D79" s="10">
+      <c r="D79" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2015,7 +2012,7 @@
       <c r="C80" s="1">
         <v>45815</v>
       </c>
-      <c r="D80" s="10">
+      <c r="D80" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2026,7 +2023,7 @@
       <c r="C81" s="1">
         <v>45816</v>
       </c>
-      <c r="D81" s="10">
+      <c r="D81" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2037,7 +2034,7 @@
       <c r="C82" s="1">
         <v>45817</v>
       </c>
-      <c r="D82" s="10">
+      <c r="D82" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2048,7 +2045,7 @@
       <c r="C83" s="1">
         <v>45818</v>
       </c>
-      <c r="D83" s="10">
+      <c r="D83" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2059,7 +2056,7 @@
       <c r="C84" s="1">
         <v>45819</v>
       </c>
-      <c r="D84" s="10">
+      <c r="D84" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2070,7 +2067,7 @@
       <c r="C85" s="1">
         <v>45820</v>
       </c>
-      <c r="D85" s="10">
+      <c r="D85" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2081,7 +2078,7 @@
       <c r="C86" s="1">
         <v>45821</v>
       </c>
-      <c r="D86" s="10">
+      <c r="D86" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2092,7 +2089,7 @@
       <c r="C87" s="1">
         <v>45822</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D87" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2103,7 +2100,7 @@
       <c r="C88" s="1">
         <v>45823</v>
       </c>
-      <c r="D88" s="10">
+      <c r="D88" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2114,7 +2111,7 @@
       <c r="C89" s="1">
         <v>45824</v>
       </c>
-      <c r="D89" s="10">
+      <c r="D89" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2125,7 +2122,7 @@
       <c r="C90" s="1">
         <v>45825</v>
       </c>
-      <c r="D90" s="10">
+      <c r="D90" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2136,7 +2133,7 @@
       <c r="C91" s="1">
         <v>45826</v>
       </c>
-      <c r="D91" s="10">
+      <c r="D91" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2147,7 +2144,7 @@
       <c r="C92" s="1">
         <v>45827</v>
       </c>
-      <c r="D92" s="10">
+      <c r="D92" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2158,7 +2155,7 @@
       <c r="C93" s="1">
         <v>45828</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D93" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2169,7 +2166,7 @@
       <c r="C94" s="1">
         <v>45829</v>
       </c>
-      <c r="D94" s="10">
+      <c r="D94" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2180,7 +2177,7 @@
       <c r="C95" s="1">
         <v>45830</v>
       </c>
-      <c r="D95" s="10">
+      <c r="D95" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2191,7 +2188,7 @@
       <c r="C96" s="1">
         <v>45831</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D96" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2202,7 +2199,7 @@
       <c r="C97" s="1">
         <v>45832</v>
       </c>
-      <c r="D97" s="10">
+      <c r="D97" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2213,7 +2210,7 @@
       <c r="C98" s="1">
         <v>45833</v>
       </c>
-      <c r="D98" s="10">
+      <c r="D98" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2224,7 +2221,7 @@
       <c r="C99" s="1">
         <v>45834</v>
       </c>
-      <c r="D99" s="10">
+      <c r="D99" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2235,7 +2232,7 @@
       <c r="C100" s="1">
         <v>45835</v>
       </c>
-      <c r="D100" s="10">
+      <c r="D100" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2246,7 +2243,7 @@
       <c r="C101" s="1">
         <v>45836</v>
       </c>
-      <c r="D101" s="10">
+      <c r="D101" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2257,7 +2254,7 @@
       <c r="C102" s="1">
         <v>45837</v>
       </c>
-      <c r="D102" s="10">
+      <c r="D102" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2268,7 +2265,7 @@
       <c r="C103" s="1">
         <v>45838</v>
       </c>
-      <c r="D103" s="10">
+      <c r="D103" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2279,7 +2276,7 @@
       <c r="C104" s="1">
         <v>45839</v>
       </c>
-      <c r="D104" s="10">
+      <c r="D104" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2290,7 +2287,7 @@
       <c r="C105" s="1">
         <v>45840</v>
       </c>
-      <c r="D105" s="10">
+      <c r="D105" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2301,7 +2298,7 @@
       <c r="C106" s="1">
         <v>45841</v>
       </c>
-      <c r="D106" s="10">
+      <c r="D106" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2312,7 +2309,7 @@
       <c r="C107" s="1">
         <v>45842</v>
       </c>
-      <c r="D107" s="10">
+      <c r="D107" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2323,7 +2320,7 @@
       <c r="C108" s="1">
         <v>45843</v>
       </c>
-      <c r="D108" s="10">
+      <c r="D108" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2334,7 +2331,7 @@
       <c r="C109" s="1">
         <v>45844</v>
       </c>
-      <c r="D109" s="10">
+      <c r="D109" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2345,7 +2342,7 @@
       <c r="C110" s="1">
         <v>45845</v>
       </c>
-      <c r="D110" s="10">
+      <c r="D110" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2356,7 +2353,7 @@
       <c r="C111" s="1">
         <v>45846</v>
       </c>
-      <c r="D111" s="10">
+      <c r="D111" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2367,7 +2364,7 @@
       <c r="C112" s="1">
         <v>45847</v>
       </c>
-      <c r="D112" s="10">
+      <c r="D112" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2378,7 +2375,7 @@
       <c r="C113" s="1">
         <v>45849</v>
       </c>
-      <c r="D113" s="10">
+      <c r="D113" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2389,7 +2386,7 @@
       <c r="C114" s="1">
         <v>45850</v>
       </c>
-      <c r="D114" s="10">
+      <c r="D114" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2400,7 +2397,7 @@
       <c r="C115" s="1">
         <v>45851</v>
       </c>
-      <c r="D115" s="10">
+      <c r="D115" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2411,7 +2408,7 @@
       <c r="C116" s="1">
         <v>45852</v>
       </c>
-      <c r="D116" s="10">
+      <c r="D116" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2422,7 +2419,7 @@
       <c r="C117" s="1">
         <v>45853</v>
       </c>
-      <c r="D117" s="10">
+      <c r="D117" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2433,7 +2430,7 @@
       <c r="C118" s="1">
         <v>45854</v>
       </c>
-      <c r="D118" s="10">
+      <c r="D118" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2444,7 +2441,7 @@
       <c r="C119" s="1">
         <v>45855</v>
       </c>
-      <c r="D119" s="10">
+      <c r="D119" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2455,7 +2452,7 @@
       <c r="C120" s="1">
         <v>45856</v>
       </c>
-      <c r="D120" s="10">
+      <c r="D120" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2466,7 +2463,7 @@
       <c r="C121" s="1">
         <v>45857</v>
       </c>
-      <c r="D121" s="10">
+      <c r="D121" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2477,7 +2474,7 @@
       <c r="C122" s="1">
         <v>45858</v>
       </c>
-      <c r="D122" s="10">
+      <c r="D122" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2488,7 +2485,7 @@
       <c r="C123" s="1">
         <v>45859</v>
       </c>
-      <c r="D123" s="10">
+      <c r="D123" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2499,7 +2496,7 @@
       <c r="C124" s="1">
         <v>45860</v>
       </c>
-      <c r="D124" s="10">
+      <c r="D124" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2510,7 +2507,7 @@
       <c r="C125" s="1">
         <v>45861</v>
       </c>
-      <c r="D125" s="10">
+      <c r="D125" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2521,7 +2518,7 @@
       <c r="C126" s="1">
         <v>45862</v>
       </c>
-      <c r="D126" s="10">
+      <c r="D126" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2532,7 +2529,7 @@
       <c r="C127" s="1">
         <v>45863</v>
       </c>
-      <c r="D127" s="10">
+      <c r="D127" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2543,7 +2540,7 @@
       <c r="C128" s="1">
         <v>45864</v>
       </c>
-      <c r="D128" s="10">
+      <c r="D128" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2554,7 +2551,7 @@
       <c r="C129" s="1">
         <v>45865</v>
       </c>
-      <c r="D129" s="10">
+      <c r="D129" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2565,7 +2562,7 @@
       <c r="C130" s="1">
         <v>45867</v>
       </c>
-      <c r="D130" s="10">
+      <c r="D130" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2576,7 +2573,7 @@
       <c r="C131" s="1">
         <v>45868</v>
       </c>
-      <c r="D131" s="10">
+      <c r="D131" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2587,7 +2584,7 @@
       <c r="C132" s="1">
         <v>45869</v>
       </c>
-      <c r="D132" s="10">
+      <c r="D132" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2598,7 +2595,7 @@
       <c r="C133" s="1">
         <v>45870</v>
       </c>
-      <c r="D133" s="10">
+      <c r="D133" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2609,7 +2606,7 @@
       <c r="C134" s="1">
         <v>45871</v>
       </c>
-      <c r="D134" s="10">
+      <c r="D134" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2620,7 +2617,7 @@
       <c r="C135" s="1">
         <v>45872</v>
       </c>
-      <c r="D135" s="10">
+      <c r="D135" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2631,7 +2628,7 @@
       <c r="C136" s="1">
         <v>45873</v>
       </c>
-      <c r="D136" s="10">
+      <c r="D136" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2642,7 +2639,7 @@
       <c r="C137" s="1">
         <v>45874</v>
       </c>
-      <c r="D137" s="10">
+      <c r="D137" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2653,7 +2650,7 @@
       <c r="C138" s="1">
         <v>45875</v>
       </c>
-      <c r="D138" s="10">
+      <c r="D138" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2664,7 +2661,7 @@
       <c r="C139" s="1">
         <v>45876</v>
       </c>
-      <c r="D139" s="10">
+      <c r="D139" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2675,7 +2672,7 @@
       <c r="C140" s="1">
         <v>45877</v>
       </c>
-      <c r="D140" s="10">
+      <c r="D140" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2686,7 +2683,7 @@
       <c r="C141" s="1">
         <v>45878</v>
       </c>
-      <c r="D141" s="10">
+      <c r="D141" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2697,7 +2694,7 @@
       <c r="C142" s="1">
         <v>45879</v>
       </c>
-      <c r="D142" s="10">
+      <c r="D142" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2708,7 +2705,7 @@
       <c r="C143" s="1">
         <v>45880</v>
       </c>
-      <c r="D143" s="10">
+      <c r="D143" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2719,7 +2716,7 @@
       <c r="C144" s="1">
         <v>45881</v>
       </c>
-      <c r="D144" s="10">
+      <c r="D144" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2730,7 +2727,7 @@
       <c r="C145" s="1">
         <v>45882</v>
       </c>
-      <c r="D145" s="10">
+      <c r="D145" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2741,7 +2738,7 @@
       <c r="C146" s="1">
         <v>45883</v>
       </c>
-      <c r="D146" s="10">
+      <c r="D146" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2752,7 +2749,7 @@
       <c r="C147" s="1">
         <v>45884</v>
       </c>
-      <c r="D147" s="10">
+      <c r="D147" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2763,7 +2760,7 @@
       <c r="C148" s="1">
         <v>45885</v>
       </c>
-      <c r="D148" s="10">
+      <c r="D148" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2774,7 +2771,7 @@
       <c r="C149" s="1">
         <v>45886</v>
       </c>
-      <c r="D149" s="10">
+      <c r="D149" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2785,7 +2782,7 @@
       <c r="C150" s="1">
         <v>45887</v>
       </c>
-      <c r="D150" s="10">
+      <c r="D150" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2796,7 +2793,7 @@
       <c r="C151" s="1">
         <v>45889</v>
       </c>
-      <c r="D151" s="10">
+      <c r="D151" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2807,7 +2804,7 @@
       <c r="C152" s="1">
         <v>45890</v>
       </c>
-      <c r="D152" s="10">
+      <c r="D152" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2818,7 +2815,7 @@
       <c r="C153" s="1">
         <v>45891</v>
       </c>
-      <c r="D153" s="10">
+      <c r="D153" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2829,7 +2826,7 @@
       <c r="C154" s="1">
         <v>45892</v>
       </c>
-      <c r="D154" s="10">
+      <c r="D154" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2840,7 +2837,7 @@
       <c r="C155" s="1">
         <v>45893</v>
       </c>
-      <c r="D155" s="10">
+      <c r="D155" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2851,7 +2848,7 @@
       <c r="C156" s="1">
         <v>45894</v>
       </c>
-      <c r="D156" s="10">
+      <c r="D156" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2862,7 +2859,7 @@
       <c r="C157" s="1">
         <v>45895</v>
       </c>
-      <c r="D157" s="10">
+      <c r="D157" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2873,7 +2870,7 @@
       <c r="C158" s="1">
         <v>45896</v>
       </c>
-      <c r="D158" s="10">
+      <c r="D158" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2884,7 +2881,7 @@
       <c r="C159" s="1">
         <v>45897</v>
       </c>
-      <c r="D159" s="10">
+      <c r="D159" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2895,7 +2892,7 @@
       <c r="C160" s="1">
         <v>45898</v>
       </c>
-      <c r="D160" s="10">
+      <c r="D160" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2906,7 +2903,7 @@
       <c r="C161" s="1">
         <v>45899</v>
       </c>
-      <c r="D161" s="10">
+      <c r="D161" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2917,7 +2914,7 @@
       <c r="C162" s="1">
         <v>45900</v>
       </c>
-      <c r="D162" s="10">
+      <c r="D162" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2928,7 +2925,7 @@
       <c r="C163" s="1">
         <v>45901</v>
       </c>
-      <c r="D163" s="10">
+      <c r="D163" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2939,7 +2936,7 @@
       <c r="C164" s="1">
         <v>45902</v>
       </c>
-      <c r="D164" s="10">
+      <c r="D164" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2950,7 +2947,7 @@
       <c r="C165" s="1">
         <v>45903</v>
       </c>
-      <c r="D165" s="10">
+      <c r="D165" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2961,7 +2958,7 @@
       <c r="C166" s="1">
         <v>45904</v>
       </c>
-      <c r="D166" s="10">
+      <c r="D166" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2972,7 +2969,7 @@
       <c r="C167" s="1">
         <v>45905</v>
       </c>
-      <c r="D167" s="10">
+      <c r="D167" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2983,7 +2980,7 @@
       <c r="C168" s="1">
         <v>45906</v>
       </c>
-      <c r="D168" s="10">
+      <c r="D168" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2994,7 +2991,7 @@
       <c r="C169" s="1">
         <v>45907</v>
       </c>
-      <c r="D169" s="10">
+      <c r="D169" s="9">
         <v>1</v>
       </c>
     </row>
@@ -3007,23 +3004,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100973BFEFB9E8EED45AA48D1DFC8B704A3" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="14a1a0664cbda954ca01f9d2f8c011fb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="593409efaa4f8321f54aa25819fe6958" ns3:_="">
     <xsd:import namespace="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
@@ -3205,31 +3185,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ABCFA1F-873A-41CD-AA3C-1BBBF10BD761}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{462615A1-65E3-4807-B3D0-35FD2C05D851}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D215757C-307E-476A-BD5E-99DFF69C32E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3245,4 +3218,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{462615A1-65E3-4807-B3D0-35FD2C05D851}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ABCFA1F-873A-41CD-AA3C-1BBBF10BD761}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
antes de rellenar <sub-subíndices>
</commit_message>
<xml_diff>
--- a/Basededatos/ECC.xlsx
+++ b/Basededatos/ECC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{E1E9DAAB-6A72-4B92-9416-19E46066190C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B7439098-DFFB-45FE-8262-A475882708A8}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{E1E9DAAB-6A72-4B92-9416-19E46066190C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{EFEFE449-A207-4448-897C-02EB4DDFE81A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{1994ACD4-0C07-4C23-B301-0329DFC64F6C}"/>
   </bookViews>
@@ -1138,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE0B658-07F5-429E-B9B4-F546CF5D0E7A}">
   <dimension ref="B2:D169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D169"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,9 +1165,7 @@
       <c r="C3" s="1">
         <v>45695</v>
       </c>
-      <c r="D3" s="8">
-        <v>4</v>
-      </c>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1176,9 +1174,7 @@
       <c r="C4" s="1">
         <v>44423</v>
       </c>
-      <c r="D4" s="8">
-        <v>4</v>
-      </c>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1187,9 +1183,7 @@
       <c r="C5" s="2">
         <v>45729</v>
       </c>
-      <c r="D5" s="8">
-        <v>4</v>
-      </c>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -1198,9 +1192,7 @@
       <c r="C6" s="1">
         <v>45741</v>
       </c>
-      <c r="D6" s="8">
-        <v>4</v>
-      </c>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -1209,9 +1201,7 @@
       <c r="C7" s="1">
         <v>45741</v>
       </c>
-      <c r="D7" s="9">
-        <v>1</v>
-      </c>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -1220,9 +1210,7 @@
       <c r="C8" s="1">
         <v>45742</v>
       </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -1231,9 +1219,7 @@
       <c r="C9" s="1">
         <v>45743</v>
       </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1242,9 +1228,7 @@
       <c r="C10" s="1">
         <v>45744</v>
       </c>
-      <c r="D10" s="9">
-        <v>1</v>
-      </c>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -1253,9 +1237,7 @@
       <c r="C11" s="1">
         <v>45745</v>
       </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -1264,9 +1246,7 @@
       <c r="C12" s="1">
         <v>45746</v>
       </c>
-      <c r="D12" s="9">
-        <v>1</v>
-      </c>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -1275,9 +1255,7 @@
       <c r="C13" s="1">
         <v>45747</v>
       </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
@@ -1286,9 +1264,7 @@
       <c r="C14" s="1">
         <v>45748</v>
       </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -1297,9 +1273,7 @@
       <c r="C15" s="1">
         <v>45749</v>
       </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
@@ -1308,9 +1282,7 @@
       <c r="C16" s="1">
         <v>45750</v>
       </c>
-      <c r="D16" s="9">
-        <v>1</v>
-      </c>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
@@ -1319,9 +1291,7 @@
       <c r="C17" s="1">
         <v>45751</v>
       </c>
-      <c r="D17" s="9">
-        <v>1</v>
-      </c>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -1330,9 +1300,7 @@
       <c r="C18" s="1">
         <v>45752</v>
       </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -1341,9 +1309,7 @@
       <c r="C19" s="1">
         <v>45753</v>
       </c>
-      <c r="D19" s="9">
-        <v>1</v>
-      </c>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -1352,9 +1318,7 @@
       <c r="C20" s="1">
         <v>45754</v>
       </c>
-      <c r="D20" s="9">
-        <v>1</v>
-      </c>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
@@ -1363,9 +1327,7 @@
       <c r="C21" s="1">
         <v>45755</v>
       </c>
-      <c r="D21" s="9">
-        <v>1</v>
-      </c>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
@@ -1374,9 +1336,7 @@
       <c r="C22" s="1">
         <v>45756</v>
       </c>
-      <c r="D22" s="9">
-        <v>1</v>
-      </c>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -1385,9 +1345,7 @@
       <c r="C23" s="1">
         <v>45757</v>
       </c>
-      <c r="D23" s="9">
-        <v>1</v>
-      </c>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
@@ -1396,9 +1354,7 @@
       <c r="C24" s="1">
         <v>45758</v>
       </c>
-      <c r="D24" s="9">
-        <v>1</v>
-      </c>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -1407,9 +1363,7 @@
       <c r="C25" s="1">
         <v>45759</v>
       </c>
-      <c r="D25" s="9">
-        <v>1</v>
-      </c>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -1418,9 +1372,7 @@
       <c r="C26" s="1">
         <v>45760</v>
       </c>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -1429,9 +1381,7 @@
       <c r="C27" s="1">
         <v>45761</v>
       </c>
-      <c r="D27" s="9">
-        <v>1</v>
-      </c>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
@@ -1440,9 +1390,7 @@
       <c r="C28" s="1">
         <v>45762</v>
       </c>
-      <c r="D28" s="9">
-        <v>1</v>
-      </c>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
@@ -1451,9 +1399,7 @@
       <c r="C29" s="1">
         <v>45763</v>
       </c>
-      <c r="D29" s="9">
-        <v>1</v>
-      </c>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
@@ -1462,9 +1408,7 @@
       <c r="C30" s="1">
         <v>45764</v>
       </c>
-      <c r="D30" s="9">
-        <v>1</v>
-      </c>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
@@ -1473,9 +1417,7 @@
       <c r="C31" s="1">
         <v>45765</v>
       </c>
-      <c r="D31" s="9">
-        <v>1</v>
-      </c>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
@@ -1484,9 +1426,7 @@
       <c r="C32" s="1">
         <v>45766</v>
       </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
@@ -1495,9 +1435,7 @@
       <c r="C33" s="1">
         <v>45767</v>
       </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
@@ -1506,9 +1444,7 @@
       <c r="C34" s="1">
         <v>45768</v>
       </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
@@ -1517,9 +1453,7 @@
       <c r="C35" s="1">
         <v>45769</v>
       </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
@@ -1528,9 +1462,7 @@
       <c r="C36" s="1">
         <v>45770</v>
       </c>
-      <c r="D36" s="9">
-        <v>1</v>
-      </c>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
@@ -1539,9 +1471,7 @@
       <c r="C37" s="1">
         <v>45771</v>
       </c>
-      <c r="D37" s="9">
-        <v>1</v>
-      </c>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
@@ -1550,9 +1480,7 @@
       <c r="C38" s="1">
         <v>45772</v>
       </c>
-      <c r="D38" s="9">
-        <v>1</v>
-      </c>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
@@ -1561,9 +1489,7 @@
       <c r="C39" s="1">
         <v>45773</v>
       </c>
-      <c r="D39" s="9">
-        <v>1</v>
-      </c>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
@@ -1572,9 +1498,7 @@
       <c r="C40" s="1">
         <v>45774</v>
       </c>
-      <c r="D40" s="9">
-        <v>1</v>
-      </c>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
@@ -1583,9 +1507,7 @@
       <c r="C41" s="1">
         <v>45775</v>
       </c>
-      <c r="D41" s="9">
-        <v>1</v>
-      </c>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
@@ -1594,9 +1516,7 @@
       <c r="C42" s="1">
         <v>45776</v>
       </c>
-      <c r="D42" s="9">
-        <v>1</v>
-      </c>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
@@ -1605,9 +1525,7 @@
       <c r="C43" s="1">
         <v>45777</v>
       </c>
-      <c r="D43" s="9">
-        <v>1</v>
-      </c>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
@@ -1616,9 +1534,7 @@
       <c r="C44" s="1">
         <v>45778</v>
       </c>
-      <c r="D44" s="9">
-        <v>1</v>
-      </c>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
@@ -1627,9 +1543,7 @@
       <c r="C45" s="1">
         <v>45779</v>
       </c>
-      <c r="D45" s="9">
-        <v>1</v>
-      </c>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
@@ -1638,9 +1552,7 @@
       <c r="C46" s="1">
         <v>45780</v>
       </c>
-      <c r="D46" s="9">
-        <v>1</v>
-      </c>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
@@ -1649,9 +1561,7 @@
       <c r="C47" s="1">
         <v>45781</v>
       </c>
-      <c r="D47" s="9">
-        <v>1</v>
-      </c>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
@@ -1660,9 +1570,7 @@
       <c r="C48" s="1">
         <v>45782</v>
       </c>
-      <c r="D48" s="9">
-        <v>1</v>
-      </c>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
@@ -1671,9 +1579,7 @@
       <c r="C49" s="1">
         <v>45783</v>
       </c>
-      <c r="D49" s="9">
-        <v>1</v>
-      </c>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
@@ -1682,9 +1588,7 @@
       <c r="C50" s="1">
         <v>45784</v>
       </c>
-      <c r="D50" s="9">
-        <v>1</v>
-      </c>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
@@ -1693,9 +1597,7 @@
       <c r="C51" s="1">
         <v>45785</v>
       </c>
-      <c r="D51" s="9">
-        <v>1</v>
-      </c>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="5">
@@ -1704,9 +1606,7 @@
       <c r="C52" s="1">
         <v>45786</v>
       </c>
-      <c r="D52" s="9">
-        <v>1</v>
-      </c>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
@@ -1715,9 +1615,7 @@
       <c r="C53" s="1">
         <v>45787</v>
       </c>
-      <c r="D53" s="9">
-        <v>1</v>
-      </c>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
@@ -1726,9 +1624,7 @@
       <c r="C54" s="1">
         <v>45788</v>
       </c>
-      <c r="D54" s="9">
-        <v>1</v>
-      </c>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
@@ -1737,9 +1633,7 @@
       <c r="C55" s="1">
         <v>45789</v>
       </c>
-      <c r="D55" s="9">
-        <v>1</v>
-      </c>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
@@ -1748,9 +1642,7 @@
       <c r="C56" s="1">
         <v>45790</v>
       </c>
-      <c r="D56" s="9">
-        <v>1</v>
-      </c>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
@@ -1759,9 +1651,7 @@
       <c r="C57" s="1">
         <v>45791</v>
       </c>
-      <c r="D57" s="9">
-        <v>1</v>
-      </c>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
@@ -1770,9 +1660,7 @@
       <c r="C58" s="1">
         <v>45792</v>
       </c>
-      <c r="D58" s="9">
-        <v>1</v>
-      </c>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
@@ -1781,9 +1669,7 @@
       <c r="C59" s="1">
         <v>45793</v>
       </c>
-      <c r="D59" s="9">
-        <v>1</v>
-      </c>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
@@ -1792,9 +1678,7 @@
       <c r="C60" s="1">
         <v>45794</v>
       </c>
-      <c r="D60" s="9">
-        <v>1</v>
-      </c>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
@@ -1803,9 +1687,7 @@
       <c r="C61" s="1">
         <v>45795</v>
       </c>
-      <c r="D61" s="9">
-        <v>1</v>
-      </c>
+      <c r="D61" s="9"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
@@ -1814,9 +1696,7 @@
       <c r="C62" s="1">
         <v>45796</v>
       </c>
-      <c r="D62" s="9">
-        <v>1</v>
-      </c>
+      <c r="D62" s="9"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="4">
@@ -1825,9 +1705,7 @@
       <c r="C63" s="1">
         <v>45797</v>
       </c>
-      <c r="D63" s="9">
-        <v>1</v>
-      </c>
+      <c r="D63" s="9"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
@@ -1836,9 +1714,7 @@
       <c r="C64" s="1">
         <v>45798</v>
       </c>
-      <c r="D64" s="9">
-        <v>1</v>
-      </c>
+      <c r="D64" s="9"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
@@ -1847,9 +1723,7 @@
       <c r="C65" s="1">
         <v>45799</v>
       </c>
-      <c r="D65" s="9">
-        <v>1</v>
-      </c>
+      <c r="D65" s="9"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
@@ -1858,9 +1732,7 @@
       <c r="C66" s="1">
         <v>45800</v>
       </c>
-      <c r="D66" s="9">
-        <v>1</v>
-      </c>
+      <c r="D66" s="9"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
@@ -1869,9 +1741,7 @@
       <c r="C67" s="1">
         <v>45801</v>
       </c>
-      <c r="D67" s="9">
-        <v>1</v>
-      </c>
+      <c r="D67" s="9"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="4">
@@ -1880,9 +1750,7 @@
       <c r="C68" s="1">
         <v>45803</v>
       </c>
-      <c r="D68" s="9">
-        <v>1</v>
-      </c>
+      <c r="D68" s="9"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="5">
@@ -1891,9 +1759,7 @@
       <c r="C69" s="1">
         <v>45804</v>
       </c>
-      <c r="D69" s="9">
-        <v>1</v>
-      </c>
+      <c r="D69" s="9"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
@@ -1902,9 +1768,7 @@
       <c r="C70" s="1">
         <v>45805</v>
       </c>
-      <c r="D70" s="9">
-        <v>1</v>
-      </c>
+      <c r="D70" s="9"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
@@ -1913,9 +1777,7 @@
       <c r="C71" s="1">
         <v>45806</v>
       </c>
-      <c r="D71" s="9">
-        <v>1</v>
-      </c>
+      <c r="D71" s="9"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
@@ -1924,9 +1786,7 @@
       <c r="C72" s="1">
         <v>45807</v>
       </c>
-      <c r="D72" s="9">
-        <v>1</v>
-      </c>
+      <c r="D72" s="9"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
@@ -1935,9 +1795,7 @@
       <c r="C73" s="1">
         <v>45808</v>
       </c>
-      <c r="D73" s="9">
-        <v>1</v>
-      </c>
+      <c r="D73" s="9"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
@@ -1946,9 +1804,7 @@
       <c r="C74" s="1">
         <v>45809</v>
       </c>
-      <c r="D74" s="9">
-        <v>1</v>
-      </c>
+      <c r="D74" s="9"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
@@ -1957,9 +1813,7 @@
       <c r="C75" s="1">
         <v>45810</v>
       </c>
-      <c r="D75" s="9">
-        <v>1</v>
-      </c>
+      <c r="D75" s="9"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
@@ -1968,9 +1822,7 @@
       <c r="C76" s="1">
         <v>45811</v>
       </c>
-      <c r="D76" s="9">
-        <v>1</v>
-      </c>
+      <c r="D76" s="9"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
@@ -1979,9 +1831,7 @@
       <c r="C77" s="1">
         <v>45812</v>
       </c>
-      <c r="D77" s="9">
-        <v>1</v>
-      </c>
+      <c r="D77" s="9"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
@@ -1990,9 +1840,7 @@
       <c r="C78" s="1">
         <v>45813</v>
       </c>
-      <c r="D78" s="9">
-        <v>1</v>
-      </c>
+      <c r="D78" s="9"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
@@ -2001,9 +1849,7 @@
       <c r="C79" s="1">
         <v>45814</v>
       </c>
-      <c r="D79" s="9">
-        <v>1</v>
-      </c>
+      <c r="D79" s="9"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
@@ -2012,9 +1858,7 @@
       <c r="C80" s="1">
         <v>45815</v>
       </c>
-      <c r="D80" s="9">
-        <v>1</v>
-      </c>
+      <c r="D80" s="9"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
@@ -2023,9 +1867,7 @@
       <c r="C81" s="1">
         <v>45816</v>
       </c>
-      <c r="D81" s="9">
-        <v>1</v>
-      </c>
+      <c r="D81" s="9"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
@@ -2034,9 +1876,7 @@
       <c r="C82" s="1">
         <v>45817</v>
       </c>
-      <c r="D82" s="9">
-        <v>1</v>
-      </c>
+      <c r="D82" s="9"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="5">
@@ -2045,9 +1885,7 @@
       <c r="C83" s="1">
         <v>45818</v>
       </c>
-      <c r="D83" s="9">
-        <v>1</v>
-      </c>
+      <c r="D83" s="9"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
@@ -2056,9 +1894,7 @@
       <c r="C84" s="1">
         <v>45819</v>
       </c>
-      <c r="D84" s="9">
-        <v>1</v>
-      </c>
+      <c r="D84" s="9"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
@@ -2067,9 +1903,7 @@
       <c r="C85" s="1">
         <v>45820</v>
       </c>
-      <c r="D85" s="9">
-        <v>1</v>
-      </c>
+      <c r="D85" s="9"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="s">
@@ -2078,9 +1912,7 @@
       <c r="C86" s="1">
         <v>45821</v>
       </c>
-      <c r="D86" s="9">
-        <v>1</v>
-      </c>
+      <c r="D86" s="9"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
@@ -2089,9 +1921,7 @@
       <c r="C87" s="1">
         <v>45822</v>
       </c>
-      <c r="D87" s="9">
-        <v>1</v>
-      </c>
+      <c r="D87" s="9"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
@@ -2100,9 +1930,7 @@
       <c r="C88" s="1">
         <v>45823</v>
       </c>
-      <c r="D88" s="9">
-        <v>1</v>
-      </c>
+      <c r="D88" s="9"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
@@ -2111,9 +1939,7 @@
       <c r="C89" s="1">
         <v>45824</v>
       </c>
-      <c r="D89" s="9">
-        <v>1</v>
-      </c>
+      <c r="D89" s="9"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
@@ -2122,9 +1948,7 @@
       <c r="C90" s="1">
         <v>45825</v>
       </c>
-      <c r="D90" s="9">
-        <v>1</v>
-      </c>
+      <c r="D90" s="9"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
@@ -2133,9 +1957,7 @@
       <c r="C91" s="1">
         <v>45826</v>
       </c>
-      <c r="D91" s="9">
-        <v>1</v>
-      </c>
+      <c r="D91" s="9"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
@@ -2144,9 +1966,7 @@
       <c r="C92" s="1">
         <v>45827</v>
       </c>
-      <c r="D92" s="9">
-        <v>1</v>
-      </c>
+      <c r="D92" s="9"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
@@ -2155,9 +1975,7 @@
       <c r="C93" s="1">
         <v>45828</v>
       </c>
-      <c r="D93" s="9">
-        <v>1</v>
-      </c>
+      <c r="D93" s="9"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
@@ -2166,9 +1984,7 @@
       <c r="C94" s="1">
         <v>45829</v>
       </c>
-      <c r="D94" s="9">
-        <v>1</v>
-      </c>
+      <c r="D94" s="9"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
@@ -2177,9 +1993,7 @@
       <c r="C95" s="1">
         <v>45830</v>
       </c>
-      <c r="D95" s="9">
-        <v>1</v>
-      </c>
+      <c r="D95" s="9"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
@@ -2188,9 +2002,7 @@
       <c r="C96" s="1">
         <v>45831</v>
       </c>
-      <c r="D96" s="9">
-        <v>1</v>
-      </c>
+      <c r="D96" s="9"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
@@ -2199,9 +2011,7 @@
       <c r="C97" s="1">
         <v>45832</v>
       </c>
-      <c r="D97" s="9">
-        <v>1</v>
-      </c>
+      <c r="D97" s="9"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="s">
@@ -2210,9 +2020,7 @@
       <c r="C98" s="1">
         <v>45833</v>
       </c>
-      <c r="D98" s="9">
-        <v>1</v>
-      </c>
+      <c r="D98" s="9"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="5">
@@ -2221,9 +2029,7 @@
       <c r="C99" s="1">
         <v>45834</v>
       </c>
-      <c r="D99" s="9">
-        <v>1</v>
-      </c>
+      <c r="D99" s="9"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
@@ -2232,9 +2038,7 @@
       <c r="C100" s="1">
         <v>45835</v>
       </c>
-      <c r="D100" s="9">
-        <v>1</v>
-      </c>
+      <c r="D100" s="9"/>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
@@ -2243,9 +2047,7 @@
       <c r="C101" s="1">
         <v>45836</v>
       </c>
-      <c r="D101" s="9">
-        <v>1</v>
-      </c>
+      <c r="D101" s="9"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
@@ -2254,9 +2056,7 @@
       <c r="C102" s="1">
         <v>45837</v>
       </c>
-      <c r="D102" s="9">
-        <v>1</v>
-      </c>
+      <c r="D102" s="9"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
@@ -2265,9 +2065,7 @@
       <c r="C103" s="1">
         <v>45838</v>
       </c>
-      <c r="D103" s="9">
-        <v>1</v>
-      </c>
+      <c r="D103" s="9"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
@@ -2276,9 +2074,7 @@
       <c r="C104" s="1">
         <v>45839</v>
       </c>
-      <c r="D104" s="9">
-        <v>1</v>
-      </c>
+      <c r="D104" s="9"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
@@ -2287,9 +2083,7 @@
       <c r="C105" s="1">
         <v>45840</v>
       </c>
-      <c r="D105" s="9">
-        <v>1</v>
-      </c>
+      <c r="D105" s="9"/>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="s">
@@ -2298,9 +2092,7 @@
       <c r="C106" s="1">
         <v>45841</v>
       </c>
-      <c r="D106" s="9">
-        <v>1</v>
-      </c>
+      <c r="D106" s="9"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="5" t="s">
@@ -2309,9 +2101,7 @@
       <c r="C107" s="1">
         <v>45842</v>
       </c>
-      <c r="D107" s="9">
-        <v>1</v>
-      </c>
+      <c r="D107" s="9"/>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
@@ -2320,9 +2110,7 @@
       <c r="C108" s="1">
         <v>45843</v>
       </c>
-      <c r="D108" s="9">
-        <v>1</v>
-      </c>
+      <c r="D108" s="9"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
@@ -2331,9 +2119,7 @@
       <c r="C109" s="1">
         <v>45844</v>
       </c>
-      <c r="D109" s="9">
-        <v>1</v>
-      </c>
+      <c r="D109" s="9"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
@@ -2342,9 +2128,7 @@
       <c r="C110" s="1">
         <v>45845</v>
       </c>
-      <c r="D110" s="9">
-        <v>1</v>
-      </c>
+      <c r="D110" s="9"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
@@ -2353,9 +2137,7 @@
       <c r="C111" s="1">
         <v>45846</v>
       </c>
-      <c r="D111" s="9">
-        <v>1</v>
-      </c>
+      <c r="D111" s="9"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="s">
@@ -2364,9 +2146,7 @@
       <c r="C112" s="1">
         <v>45847</v>
       </c>
-      <c r="D112" s="9">
-        <v>1</v>
-      </c>
+      <c r="D112" s="9"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="4">
@@ -2375,9 +2155,7 @@
       <c r="C113" s="1">
         <v>45849</v>
       </c>
-      <c r="D113" s="9">
-        <v>1</v>
-      </c>
+      <c r="D113" s="9"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
@@ -2386,9 +2164,7 @@
       <c r="C114" s="1">
         <v>45850</v>
       </c>
-      <c r="D114" s="9">
-        <v>1</v>
-      </c>
+      <c r="D114" s="9"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="4" t="s">
@@ -2397,9 +2173,7 @@
       <c r="C115" s="1">
         <v>45851</v>
       </c>
-      <c r="D115" s="9">
-        <v>1</v>
-      </c>
+      <c r="D115" s="9"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
@@ -2408,9 +2182,7 @@
       <c r="C116" s="1">
         <v>45852</v>
       </c>
-      <c r="D116" s="9">
-        <v>1</v>
-      </c>
+      <c r="D116" s="9"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="4" t="s">
@@ -2419,9 +2191,7 @@
       <c r="C117" s="1">
         <v>45853</v>
       </c>
-      <c r="D117" s="9">
-        <v>1</v>
-      </c>
+      <c r="D117" s="9"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="5">
@@ -2430,9 +2200,7 @@
       <c r="C118" s="1">
         <v>45854</v>
       </c>
-      <c r="D118" s="9">
-        <v>1</v>
-      </c>
+      <c r="D118" s="9"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="4" t="s">
@@ -2441,9 +2209,7 @@
       <c r="C119" s="1">
         <v>45855</v>
       </c>
-      <c r="D119" s="9">
-        <v>1</v>
-      </c>
+      <c r="D119" s="9"/>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="5" t="s">
@@ -2452,9 +2218,7 @@
       <c r="C120" s="1">
         <v>45856</v>
       </c>
-      <c r="D120" s="9">
-        <v>1</v>
-      </c>
+      <c r="D120" s="9"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="4" t="s">
@@ -2463,9 +2227,7 @@
       <c r="C121" s="1">
         <v>45857</v>
       </c>
-      <c r="D121" s="9">
-        <v>1</v>
-      </c>
+      <c r="D121" s="9"/>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="5" t="s">
@@ -2474,9 +2236,7 @@
       <c r="C122" s="1">
         <v>45858</v>
       </c>
-      <c r="D122" s="9">
-        <v>1</v>
-      </c>
+      <c r="D122" s="9"/>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
@@ -2485,9 +2245,7 @@
       <c r="C123" s="1">
         <v>45859</v>
       </c>
-      <c r="D123" s="9">
-        <v>1</v>
-      </c>
+      <c r="D123" s="9"/>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="5" t="s">
@@ -2496,9 +2254,7 @@
       <c r="C124" s="1">
         <v>45860</v>
       </c>
-      <c r="D124" s="9">
-        <v>1</v>
-      </c>
+      <c r="D124" s="9"/>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="4">
@@ -2507,9 +2263,7 @@
       <c r="C125" s="1">
         <v>45861</v>
       </c>
-      <c r="D125" s="9">
-        <v>1</v>
-      </c>
+      <c r="D125" s="9"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="5">
@@ -2518,9 +2272,7 @@
       <c r="C126" s="1">
         <v>45862</v>
       </c>
-      <c r="D126" s="9">
-        <v>1</v>
-      </c>
+      <c r="D126" s="9"/>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="4" t="s">
@@ -2529,9 +2281,7 @@
       <c r="C127" s="1">
         <v>45863</v>
       </c>
-      <c r="D127" s="9">
-        <v>1</v>
-      </c>
+      <c r="D127" s="9"/>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="5">
@@ -2540,9 +2290,7 @@
       <c r="C128" s="1">
         <v>45864</v>
       </c>
-      <c r="D128" s="9">
-        <v>1</v>
-      </c>
+      <c r="D128" s="9"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
@@ -2551,9 +2299,7 @@
       <c r="C129" s="1">
         <v>45865</v>
       </c>
-      <c r="D129" s="9">
-        <v>1</v>
-      </c>
+      <c r="D129" s="9"/>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="6" t="s">
@@ -2562,9 +2308,7 @@
       <c r="C130" s="1">
         <v>45867</v>
       </c>
-      <c r="D130" s="9">
-        <v>1</v>
-      </c>
+      <c r="D130" s="9"/>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="5" t="s">
@@ -2573,9 +2317,7 @@
       <c r="C131" s="1">
         <v>45868</v>
       </c>
-      <c r="D131" s="9">
-        <v>1</v>
-      </c>
+      <c r="D131" s="9"/>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="4" t="s">
@@ -2584,9 +2326,7 @@
       <c r="C132" s="1">
         <v>45869</v>
       </c>
-      <c r="D132" s="9">
-        <v>1</v>
-      </c>
+      <c r="D132" s="9"/>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="5" t="s">
@@ -2595,9 +2335,7 @@
       <c r="C133" s="1">
         <v>45870</v>
       </c>
-      <c r="D133" s="9">
-        <v>1</v>
-      </c>
+      <c r="D133" s="9"/>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="4" t="s">
@@ -2606,9 +2344,7 @@
       <c r="C134" s="1">
         <v>45871</v>
       </c>
-      <c r="D134" s="9">
-        <v>1</v>
-      </c>
+      <c r="D134" s="9"/>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="5" t="s">
@@ -2617,9 +2353,7 @@
       <c r="C135" s="1">
         <v>45872</v>
       </c>
-      <c r="D135" s="9">
-        <v>1</v>
-      </c>
+      <c r="D135" s="9"/>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="4" t="s">
@@ -2628,9 +2362,7 @@
       <c r="C136" s="1">
         <v>45873</v>
       </c>
-      <c r="D136" s="9">
-        <v>1</v>
-      </c>
+      <c r="D136" s="9"/>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="5" t="s">
@@ -2639,9 +2371,7 @@
       <c r="C137" s="1">
         <v>45874</v>
       </c>
-      <c r="D137" s="9">
-        <v>1</v>
-      </c>
+      <c r="D137" s="9"/>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
@@ -2650,9 +2380,7 @@
       <c r="C138" s="1">
         <v>45875</v>
       </c>
-      <c r="D138" s="9">
-        <v>1</v>
-      </c>
+      <c r="D138" s="9"/>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="5" t="s">
@@ -2661,9 +2389,7 @@
       <c r="C139" s="1">
         <v>45876</v>
       </c>
-      <c r="D139" s="9">
-        <v>1</v>
-      </c>
+      <c r="D139" s="9"/>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="4" t="s">
@@ -2672,9 +2398,7 @@
       <c r="C140" s="1">
         <v>45877</v>
       </c>
-      <c r="D140" s="9">
-        <v>1</v>
-      </c>
+      <c r="D140" s="9"/>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="5" t="s">
@@ -2683,9 +2407,7 @@
       <c r="C141" s="1">
         <v>45878</v>
       </c>
-      <c r="D141" s="9">
-        <v>1</v>
-      </c>
+      <c r="D141" s="9"/>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="4" t="s">
@@ -2694,9 +2416,7 @@
       <c r="C142" s="1">
         <v>45879</v>
       </c>
-      <c r="D142" s="9">
-        <v>1</v>
-      </c>
+      <c r="D142" s="9"/>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="5" t="s">
@@ -2705,9 +2425,7 @@
       <c r="C143" s="1">
         <v>45880</v>
       </c>
-      <c r="D143" s="9">
-        <v>1</v>
-      </c>
+      <c r="D143" s="9"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="4" t="s">
@@ -2716,9 +2434,7 @@
       <c r="C144" s="1">
         <v>45881</v>
       </c>
-      <c r="D144" s="9">
-        <v>1</v>
-      </c>
+      <c r="D144" s="9"/>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="5" t="s">
@@ -2727,9 +2443,7 @@
       <c r="C145" s="1">
         <v>45882</v>
       </c>
-      <c r="D145" s="9">
-        <v>1</v>
-      </c>
+      <c r="D145" s="9"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
@@ -2738,9 +2452,7 @@
       <c r="C146" s="1">
         <v>45883</v>
       </c>
-      <c r="D146" s="9">
-        <v>1</v>
-      </c>
+      <c r="D146" s="9"/>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="5">
@@ -2749,9 +2461,7 @@
       <c r="C147" s="1">
         <v>45884</v>
       </c>
-      <c r="D147" s="9">
-        <v>1</v>
-      </c>
+      <c r="D147" s="9"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="4" t="s">
@@ -2760,9 +2470,7 @@
       <c r="C148" s="1">
         <v>45885</v>
       </c>
-      <c r="D148" s="9">
-        <v>1</v>
-      </c>
+      <c r="D148" s="9"/>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="5">
@@ -2771,9 +2479,7 @@
       <c r="C149" s="1">
         <v>45886</v>
       </c>
-      <c r="D149" s="9">
-        <v>1</v>
-      </c>
+      <c r="D149" s="9"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="4" t="s">
@@ -2782,9 +2488,7 @@
       <c r="C150" s="1">
         <v>45887</v>
       </c>
-      <c r="D150" s="9">
-        <v>1</v>
-      </c>
+      <c r="D150" s="9"/>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
@@ -2793,9 +2497,7 @@
       <c r="C151" s="1">
         <v>45889</v>
       </c>
-      <c r="D151" s="9">
-        <v>1</v>
-      </c>
+      <c r="D151" s="9"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="5" t="s">
@@ -2804,9 +2506,7 @@
       <c r="C152" s="1">
         <v>45890</v>
       </c>
-      <c r="D152" s="9">
-        <v>1</v>
-      </c>
+      <c r="D152" s="9"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="4" t="s">
@@ -2815,9 +2515,7 @@
       <c r="C153" s="1">
         <v>45891</v>
       </c>
-      <c r="D153" s="9">
-        <v>1</v>
-      </c>
+      <c r="D153" s="9"/>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="5" t="s">
@@ -2826,9 +2524,7 @@
       <c r="C154" s="1">
         <v>45892</v>
       </c>
-      <c r="D154" s="9">
-        <v>1</v>
-      </c>
+      <c r="D154" s="9"/>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="4" t="s">
@@ -2837,9 +2533,7 @@
       <c r="C155" s="1">
         <v>45893</v>
       </c>
-      <c r="D155" s="9">
-        <v>1</v>
-      </c>
+      <c r="D155" s="9"/>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="5" t="s">
@@ -2848,9 +2542,7 @@
       <c r="C156" s="1">
         <v>45894</v>
       </c>
-      <c r="D156" s="9">
-        <v>1</v>
-      </c>
+      <c r="D156" s="9"/>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="4">
@@ -2859,9 +2551,7 @@
       <c r="C157" s="1">
         <v>45895</v>
       </c>
-      <c r="D157" s="9">
-        <v>1</v>
-      </c>
+      <c r="D157" s="9"/>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="5">
@@ -2870,9 +2560,7 @@
       <c r="C158" s="1">
         <v>45896</v>
       </c>
-      <c r="D158" s="9">
-        <v>1</v>
-      </c>
+      <c r="D158" s="9"/>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="4" t="s">
@@ -2881,9 +2569,7 @@
       <c r="C159" s="1">
         <v>45897</v>
       </c>
-      <c r="D159" s="9">
-        <v>1</v>
-      </c>
+      <c r="D159" s="9"/>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="5" t="s">
@@ -2892,9 +2578,7 @@
       <c r="C160" s="1">
         <v>45898</v>
       </c>
-      <c r="D160" s="9">
-        <v>1</v>
-      </c>
+      <c r="D160" s="9"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="4" t="s">
@@ -2903,9 +2587,7 @@
       <c r="C161" s="1">
         <v>45899</v>
       </c>
-      <c r="D161" s="9">
-        <v>1</v>
-      </c>
+      <c r="D161" s="9"/>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" s="5" t="s">
@@ -2914,9 +2596,7 @@
       <c r="C162" s="1">
         <v>45900</v>
       </c>
-      <c r="D162" s="9">
-        <v>1</v>
-      </c>
+      <c r="D162" s="9"/>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="4" t="s">
@@ -2925,9 +2605,7 @@
       <c r="C163" s="1">
         <v>45901</v>
       </c>
-      <c r="D163" s="9">
-        <v>1</v>
-      </c>
+      <c r="D163" s="9"/>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="5" t="s">
@@ -2936,9 +2614,7 @@
       <c r="C164" s="1">
         <v>45902</v>
       </c>
-      <c r="D164" s="9">
-        <v>1</v>
-      </c>
+      <c r="D164" s="9"/>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="4" t="s">
@@ -2947,9 +2623,7 @@
       <c r="C165" s="1">
         <v>45903</v>
       </c>
-      <c r="D165" s="9">
-        <v>1</v>
-      </c>
+      <c r="D165" s="9"/>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="5" t="s">
@@ -2958,9 +2632,7 @@
       <c r="C166" s="1">
         <v>45904</v>
       </c>
-      <c r="D166" s="9">
-        <v>1</v>
-      </c>
+      <c r="D166" s="9"/>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="4" t="s">
@@ -2969,9 +2641,7 @@
       <c r="C167" s="1">
         <v>45905</v>
       </c>
-      <c r="D167" s="9">
-        <v>1</v>
-      </c>
+      <c r="D167" s="9"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="7" t="s">
@@ -2980,9 +2650,7 @@
       <c r="C168" s="1">
         <v>45906</v>
       </c>
-      <c r="D168" s="9">
-        <v>1</v>
-      </c>
+      <c r="D168" s="9"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="4" t="s">
@@ -2991,9 +2659,7 @@
       <c r="C169" s="1">
         <v>45907</v>
       </c>
-      <c r="D169" s="9">
-        <v>1</v>
-      </c>
+      <c r="D169" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3004,6 +2670,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100973BFEFB9E8EED45AA48D1DFC8B704A3" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="14a1a0664cbda954ca01f9d2f8c011fb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1cc19d0-e28e-4f1b-b120-4e42c2fee203" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="593409efaa4f8321f54aa25819fe6958" ns3:_="">
     <xsd:import namespace="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
@@ -3185,15 +2860,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3203,6 +2869,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{462615A1-65E3-4807-B3D0-35FD2C05D851}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D215757C-307E-476A-BD5E-99DFF69C32E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3220,26 +2894,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{462615A1-65E3-4807-B3D0-35FD2C05D851}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ABCFA1F-873A-41CD-AA3C-1BBBF10BD761}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>